<commit_message>
Atualização automática de 2O_GRAU.xlsx
</commit_message>
<xml_diff>
--- a/2O_GRAU.xlsx
+++ b/2O_GRAU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF1C75D1-0B38-4A07-BB81-DD0FEEC520CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{402AC8A4-6D4E-4A3B-BED4-0010AD2A256E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2023,7 +2023,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{919EB142-C90D-42F1-98E9-28FF6FD495D2}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{85FBF079-C391-4DCC-826D-9BBA66C08BE5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2053,10 +2053,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB1DC48B-F143-4AE8-A534-2E4D88409B82}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{340D92CB-2F21-45A0-9ADC-AC771B2605CB}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2094,7 +2094,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E70AFE8-C6DD-4E68-8BD1-FC2E860CA7F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EC8918E-99B2-42C8-A969-EFB4A47709BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2157,7 +2157,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A048F4CD-19AF-4663-874A-B3167A553E75}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{539A4936-8C3A-4BB5-8E9B-13C46D284FC8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2176,7 +2176,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C86753F-BB26-D290-5BE7-E6D844AFA83A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5615A783-83CA-E0F8-D094-F7CDA905C0F9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2225,7 +2225,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13BD8A62-DAFE-24B8-FC72-5002A6A0DA19}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C74E426-95EC-BEE3-52ED-048D83B0AED3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2244,7 +2244,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23D7C901-CE83-8970-96CB-FB298119ECA1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF2F4423-8583-F867-493B-1F8B3A15A429}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2275,7 +2275,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69A21A11-DED0-812B-B472-9A31E83B739B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51C857FB-39C9-B39F-9D81-1E54F1CC5490}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2306,7 +2306,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77BD9013-926E-AB9C-A5CD-575BCD4DDFB8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F424639B-E013-33CF-7C54-279ABAB383AB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2349,7 +2349,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4BD1CD5-12FF-472C-A1DE-859B8F40C483}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F5BE50B-DA01-46D8-9A1F-4D69E6F0224F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2387,7 +2387,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EA88214-5D49-4E56-8236-C10CD530C32F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72D6694F-BF85-4186-A917-BF84CAD11142}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2430,7 +2430,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{380BBC3E-FA1E-4A08-83E0-E2173AA6683D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77B1162C-B9E4-4A39-80DD-CFBA71166E93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2743,7 +2743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2F98D1-86C0-4E28-9885-4BD724BC58AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F08E1CD-8184-4284-A8D0-2D4BCB66EB26}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>